<commit_message>
updated meta files for DO
</commit_message>
<xml_diff>
--- a/gl4.buoy.PMEDO.meta.xlsx
+++ b/gl4.buoy.PMEDO.meta.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellyloria/Documents/Niwot LTER 2017-2019/GL4 Sensor/Buoy Data/Buoy_QAQC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{1DA365C3-A369-4E4E-A575-8650E5376121}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{D86A39DD-E375-E64F-B3B2-AD15F79D70E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="20760" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="gl4_buyRBRTemp.meta" sheetId="2" r:id="rId2"/>
+    <sheet name="gl4_bouy.PMEDO.meta" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="disciplines">metadata!$T$2:$T$13</definedName>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="192">
   <si>
     <t>Methods:</t>
   </si>
@@ -548,15 +548,6 @@
     <t xml:space="preserve">Sensor information </t>
   </si>
   <si>
-    <t xml:space="preserve">We deployed 8 RBR temperature sensors along 13 meter deep buoy. </t>
-  </si>
-  <si>
-    <t>RBRsolo³ T are rated for ±0.002°C accuracy, &lt;0.00005°C resolution and were set to record in 30 minute intervals.</t>
-  </si>
-  <si>
-    <t>Sensors were downloaded using their interal software (ruskin).</t>
-  </si>
-  <si>
     <t>QA'QC protocol</t>
   </si>
   <si>
@@ -579,15 +570,6 @@
   </si>
   <si>
     <t>For the summer 2018 deployment, the only values that were removed corresponded with the July 10th adjustments.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Then we aggregated all individual RBRsolo³ T in r to create a master file. </t>
-  </si>
-  <si>
-    <t>The upper most sensor (0.4m) was positioned under a surface float, as to protect it from direct sunlight.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All RBR sensors were postioned vertically along the bouy with the probe side pointing downwards. </t>
   </si>
   <si>
     <t xml:space="preserve">See attatched diagram for details. </t>
@@ -645,6 +627,57 @@
   </si>
   <si>
     <t>dissolved oxygen in miligrams per liter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We deployed 3 PME MINIDOT® sensors along 13 meter deep buoy. </t>
+  </si>
+  <si>
+    <t>The disloved oxygen loggers collects measurements of dissolved oxygen with an accuracy of +/- 5% and temperature to +/- 0.1 degrees C.</t>
+  </si>
+  <si>
+    <t>Temperature range is 0 to 35 degrees C with an accuracy of +/- 0.1 degrees C.</t>
+  </si>
+  <si>
+    <t>Oxygen range is 0 to 150% saturation with an accuracy of +/- 10 umole/L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All measurements are stored internally and data is offloaded to a computer via the miniDOT USB cable. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We also calculated mean dissloved oxgen and the standard deviation of that mean. </t>
+  </si>
+  <si>
+    <t>We also looked for any temperature values outside the accuracy range of 0 to 35 degrees celcius as well as dissloved oxygen saturation outside of 0 to 150%.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then we aggregated all individual MINIDOT® data in r to create a master file. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All MINIDOT®  sensors were postioned vertically along the bouy with the probe side pointing downwards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each senor was accoumpanies by a anti-fouling wiper. </t>
+  </si>
+  <si>
+    <t>battery voltage,</t>
+  </si>
+  <si>
+    <t>volts</t>
+  </si>
+  <si>
+    <t>We also checked the batteray voltage to ensure that all measurements were recorded with atleast 1.50 volts</t>
+  </si>
+  <si>
+    <t>Lastly PME MINIDOT® sensors are equiped with a quality measurement Q, which rates idividual measurements as a ratio of the [DO] as determined from emission intensity to the [DO] as determined by emission lifetime.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideally Q should be around, 1 so we removed all measurements which contained a Q score of 0.7 or less. </t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Q is the ratio of the [DO] as determined from emission intensity to the [DO] as determined by emission lifetime.</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1815,7 +1848,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2495,10 +2528,10 @@
         <v>133</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -3107,24 +3140,24 @@
         <v>2</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E64" s="29"/>
       <c r="F64" s="44" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G64" s="44" t="s">
         <v>56</v>
       </c>
       <c r="H64" s="29"/>
       <c r="I64" s="32" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3160,7 +3193,7 @@
       </c>
       <c r="H65" s="29"/>
       <c r="I65" s="29" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -3185,7 +3218,7 @@
         <v>137</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="40">
@@ -3196,7 +3229,7 @@
       </c>
       <c r="H66" s="29"/>
       <c r="I66" s="32" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3291,13 +3324,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>137</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E69" s="29"/>
       <c r="F69" s="29">
@@ -3306,9 +3339,11 @@
       <c r="G69" s="29">
         <v>8.4529999999999994</v>
       </c>
-      <c r="H69" s="29"/>
+      <c r="H69" s="29">
+        <v>0.01</v>
+      </c>
       <c r="I69" s="29" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3327,11 +3362,11 @@
         <v>8</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C70" s="29"/>
       <c r="D70" s="29" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E70" s="29"/>
       <c r="F70" s="45">
@@ -3340,7 +3375,9 @@
       <c r="G70" s="45">
         <v>111.25</v>
       </c>
-      <c r="H70" s="29"/>
+      <c r="H70" s="29">
+        <v>5</v>
+      </c>
       <c r="I70" s="29"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -3359,10 +3396,14 @@
         <v>9</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
-      <c r="C71" s="29"/>
-      <c r="D71" s="29"/>
+      <c r="C71" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>186</v>
+      </c>
       <c r="E71" s="29"/>
       <c r="F71" s="29">
         <v>3.41</v>
@@ -3371,7 +3412,9 @@
         <v>3.5</v>
       </c>
       <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
+      <c r="I71" s="29" t="s">
+        <v>185</v>
+      </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
@@ -3389,10 +3432,14 @@
         <v>10</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
-      <c r="C72" s="29"/>
-      <c r="D72" s="29"/>
+      <c r="C72" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="E72" s="29"/>
       <c r="F72" s="29">
         <v>0.96399999999999997</v>
@@ -3401,7 +3448,9 @@
         <v>1.0309999999999999</v>
       </c>
       <c r="H72" s="29"/>
-      <c r="I72" s="29"/>
+      <c r="I72" s="29" t="s">
+        <v>191</v>
+      </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
@@ -23872,10 +23921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H982"/>
+  <dimension ref="A1:H989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24049,7 +24098,7 @@
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -24061,7 +24110,7 @@
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -24073,7 +24122,7 @@
     </row>
     <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -24084,7 +24133,9 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -24093,32 +24144,14 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
-        <v>151</v>
+    <row r="19" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="33" t="s">
+        <v>179</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
+    </row>
+    <row r="20" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="30" t="s">
-        <v>152</v>
-      </c>
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -24128,8 +24161,8 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="33" t="s">
-        <v>153</v>
+      <c r="A22" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -24140,8 +24173,8 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="33" t="s">
-        <v>155</v>
+      <c r="A23" s="30" t="s">
+        <v>149</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -24153,7 +24186,7 @@
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="33" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -24165,7 +24198,7 @@
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -24177,7 +24210,7 @@
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="33" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -24189,7 +24222,7 @@
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="33" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -24199,20 +24232,15 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="33" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2"/>
+      <c r="A29" s="33" t="s">
+        <v>154</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -24221,56 +24249,30 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="8" t="s">
-        <v>59</v>
+    <row r="30" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="33" t="s">
+        <v>181</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="30" t="s">
-        <v>160</v>
+    </row>
+    <row r="31" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="33" t="s">
+        <v>187</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="30" t="s">
-        <v>161</v>
+    </row>
+    <row r="32" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="33" t="s">
+        <v>188</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="30" t="s">
-        <v>162</v>
+    </row>
+    <row r="33" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="33" t="s">
+        <v>189</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2"/>
+      <c r="A34" s="33" t="s">
+        <v>155</v>
+      </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -24280,7 +24282,9 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2"/>
+      <c r="A35" s="33" t="s">
+        <v>182</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -24290,7 +24294,7 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="33"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -24300,7 +24304,9 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2"/>
+      <c r="A37" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -24310,7 +24316,9 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2"/>
+      <c r="A38" s="33" t="s">
+        <v>183</v>
+      </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -24319,18 +24327,15 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+    <row r="39" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="33" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2"/>
+      <c r="A40" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -24340,7 +24345,7 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="13"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -24350,7 +24355,7 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="13"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -24360,7 +24365,7 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="13"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -24370,7 +24375,7 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="13"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -24380,7 +24385,7 @@
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="13"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -24410,7 +24415,7 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -24420,7 +24425,7 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -24430,7 +24435,7 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="2"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -24440,7 +24445,7 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -24450,7 +24455,7 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="2"/>
+      <c r="A52" s="13"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -33759,6 +33764,76 @@
       <c r="G982" s="2"/>
       <c r="H982" s="2"/>
     </row>
+    <row r="983" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A983" s="2"/>
+      <c r="B983" s="2"/>
+      <c r="C983" s="2"/>
+      <c r="D983" s="2"/>
+      <c r="E983" s="2"/>
+      <c r="F983" s="2"/>
+      <c r="G983" s="2"/>
+      <c r="H983" s="2"/>
+    </row>
+    <row r="984" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A984" s="2"/>
+      <c r="B984" s="2"/>
+      <c r="C984" s="2"/>
+      <c r="D984" s="2"/>
+      <c r="E984" s="2"/>
+      <c r="F984" s="2"/>
+      <c r="G984" s="2"/>
+      <c r="H984" s="2"/>
+    </row>
+    <row r="985" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A985" s="2"/>
+      <c r="B985" s="2"/>
+      <c r="C985" s="2"/>
+      <c r="D985" s="2"/>
+      <c r="E985" s="2"/>
+      <c r="F985" s="2"/>
+      <c r="G985" s="2"/>
+      <c r="H985" s="2"/>
+    </row>
+    <row r="986" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A986" s="2"/>
+      <c r="B986" s="2"/>
+      <c r="C986" s="2"/>
+      <c r="D986" s="2"/>
+      <c r="E986" s="2"/>
+      <c r="F986" s="2"/>
+      <c r="G986" s="2"/>
+      <c r="H986" s="2"/>
+    </row>
+    <row r="987" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A987" s="2"/>
+      <c r="B987" s="2"/>
+      <c r="C987" s="2"/>
+      <c r="D987" s="2"/>
+      <c r="E987" s="2"/>
+      <c r="F987" s="2"/>
+      <c r="G987" s="2"/>
+      <c r="H987" s="2"/>
+    </row>
+    <row r="988" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A988" s="2"/>
+      <c r="B988" s="2"/>
+      <c r="C988" s="2"/>
+      <c r="D988" s="2"/>
+      <c r="E988" s="2"/>
+      <c r="F988" s="2"/>
+      <c r="G988" s="2"/>
+      <c r="H988" s="2"/>
+    </row>
+    <row r="989" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A989" s="2"/>
+      <c r="B989" s="2"/>
+      <c r="C989" s="2"/>
+      <c r="D989" s="2"/>
+      <c r="E989" s="2"/>
+      <c r="F989" s="2"/>
+      <c r="G989" s="2"/>
+      <c r="H989" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Spell checked meta data.
</commit_message>
<xml_diff>
--- a/gl4.buoy.PMEDO.meta.xlsx
+++ b/gl4.buoy.PMEDO.meta.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellyloria/Documents/Niwot LTER 2017-2019/GL4 Sensor/Buoy Data/Buoy_QAQC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF290450-A165-5540-8C98-0D9B028AD159}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073D4C83-3791-6C41-BA50-6C94DC02888B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="20760" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="gl4_bouy.PMEDO.meta" sheetId="2" r:id="rId2"/>
+    <sheet name="gl4_buoy.PMEDO.meta" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="disciplines">metadata!$T$2:$T$13</definedName>
@@ -554,25 +554,10 @@
     <t xml:space="preserve">Individual sensor output was QA'Qced in R. </t>
   </si>
   <si>
-    <t xml:space="preserve">First date range was restricted around deployement record to exclude and measurements taken while the buoy was being manipulated. </t>
-  </si>
-  <si>
     <t>Then timestamps were checked to make sure there were no duplicates.</t>
   </si>
   <si>
     <t>For 2018 summer deployment, measurements were restricted to the date range '2018-07-03 13:00:00' to '2018-08-21 00:00:00'.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Next we calculated mean temperature and the standard deviation of that mean. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">We removed any values that were more than 3 deviations away from the mean for a given sensor. </t>
-  </si>
-  <si>
-    <t>For the summer 2018 deployment, the only values that were removed corresponded with the July 10th adjustments.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See attatched diagram for details. </t>
   </si>
   <si>
     <t>deployment</t>
@@ -629,9 +614,6 @@
     <t xml:space="preserve">We deployed 3 PME MINIDOT® sensors along 13 meter deep buoy. </t>
   </si>
   <si>
-    <t>The disloved oxygen loggers collects measurements of dissolved oxygen with an accuracy of +/- 5% and temperature to +/- 0.1 degrees C.</t>
-  </si>
-  <si>
     <t>Temperature range is 0 to 35 degrees C with an accuracy of +/- 0.1 degrees C.</t>
   </si>
   <si>
@@ -641,31 +623,13 @@
     <t xml:space="preserve">All measurements are stored internally and data is offloaded to a computer via the miniDOT USB cable. </t>
   </si>
   <si>
-    <t xml:space="preserve">We also calculated mean dissloved oxgen and the standard deviation of that mean. </t>
-  </si>
-  <si>
-    <t>We also looked for any temperature values outside the accuracy range of 0 to 35 degrees celcius as well as dissloved oxygen saturation outside of 0 to 150%.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Then we aggregated all individual MINIDOT® data in r to create a master file. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">All MINIDOT®  sensors were postioned vertically along the bouy with the probe side pointing downwards. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each senor was accoumpanies by a anti-fouling wiper. </t>
   </si>
   <si>
     <t>battery voltage,</t>
   </si>
   <si>
     <t>volts</t>
-  </si>
-  <si>
-    <t>We also checked the batteray voltage to ensure that all measurements were recorded with atleast 1.50 volts</t>
-  </si>
-  <si>
-    <t>Lastly PME MINIDOT® sensors are equiped with a quality measurement Q, which rates idividual measurements as a ratio of the [DO] as determined from emission intensity to the [DO] as determined by emission lifetime.</t>
   </si>
   <si>
     <t xml:space="preserve">Ideally Q should be around, 1 so we removed all measurements which contained a Q score of 0.7 or less. </t>
@@ -679,6 +643,42 @@
   <si>
     <t>gl4.buoy.PMEDO.data.csv</t>
   </si>
+  <si>
+    <t xml:space="preserve">Then we created QA'QC thresholds by multiplying the mean temperature by 3 times the standard deviation and add or subtracting that value to the  mean to create an upper and lower QA'QC threshold. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then  we restricted the data set to include only observations that fell within that the upper and lower threshold. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We repeated this step for DO measurements. </t>
+  </si>
+  <si>
+    <t>For the summer 2018 deployment,  we removed  values that corresponded with the July 10th adjustments.</t>
+  </si>
+  <si>
+    <t>The dissolved oxygen loggers collects measurements of dissolved oxygen with an accuracy of +/- 5% and temperature to +/- 0.1 degrees C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First date range was restricted around deployment record to exclude and measurements taken while the buoy was being manipulated. </t>
+  </si>
+  <si>
+    <t>We also looked for any temperature values outside the accuracy range of 0 to 35 degrees Celsius as well as dissolved oxygen saturation outside of 0 to 150%.</t>
+  </si>
+  <si>
+    <t>We checked the battery voltage to ensure that all measurements were recorded with at least 1.50 volts</t>
+  </si>
+  <si>
+    <t>PME MINIDOT® sensors are equipped with a quality measurement Q, which rates individual measurements as a ratio of the [DO] as determined from emission intensity to the [DO] as determined by emission lifetime.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All MINIDOT®  sensors were positioned vertically along the buoy with the probe side pointing downwards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each senor was accompanies by a anti-fouling wiper. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">See attached diagram for details. </t>
+  </si>
 </sst>
 </file>
 
@@ -688,7 +688,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -735,6 +735,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -936,7 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -997,10 +1003,12 @@
     <xf numFmtId="164" fontId="6" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1372,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1392,14 +1400,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1848,7 +1856,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2528,10 +2536,10 @@
         <v>133</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -3140,24 +3148,24 @@
         <v>2</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E64" s="29"/>
       <c r="F64" s="42" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G64" s="42" t="s">
         <v>56</v>
       </c>
       <c r="H64" s="29"/>
       <c r="I64" s="32" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3193,7 +3201,7 @@
       </c>
       <c r="H65" s="29"/>
       <c r="I65" s="29" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -3218,7 +3226,7 @@
         <v>137</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="40">
@@ -3229,7 +3237,7 @@
       </c>
       <c r="H66" s="29"/>
       <c r="I66" s="32" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3324,13 +3332,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>137</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E69" s="29"/>
       <c r="F69" s="29">
@@ -3343,7 +3351,7 @@
         <v>0.01</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3362,11 +3370,11 @@
         <v>8</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C70" s="29"/>
       <c r="D70" s="29" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E70" s="29"/>
       <c r="F70" s="43">
@@ -3396,13 +3404,13 @@
         <v>9</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C71" s="32" t="s">
         <v>137</v>
       </c>
       <c r="D71" s="32" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E71" s="29"/>
       <c r="F71" s="29">
@@ -3413,7 +3421,7 @@
       </c>
       <c r="H71" s="29"/>
       <c r="I71" s="29" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -3432,13 +3440,13 @@
         <v>10</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C72" s="32" t="s">
         <v>137</v>
       </c>
       <c r="D72" s="32" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E72" s="29"/>
       <c r="F72" s="29">
@@ -3449,7 +3457,7 @@
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="29" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -23923,8 +23931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24098,7 +24106,7 @@
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -24110,7 +24118,7 @@
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -24122,7 +24130,7 @@
     </row>
     <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -24133,8 +24141,8 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>177</v>
+      <c r="A18" s="33" t="s">
+        <v>171</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -24146,7 +24154,7 @@
     </row>
     <row r="19" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="33" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24186,7 +24194,7 @@
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="33" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -24198,7 +24206,7 @@
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -24208,21 +24216,14 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="33" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -24234,56 +24235,42 @@
     </row>
     <row r="28" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="33" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="33" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="47" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="33" t="s">
-        <v>186</v>
+    <row r="33" spans="1:8" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="47" t="s">
+        <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="33" t="s">
-        <v>187</v>
+    <row r="34" spans="1:8" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="47" t="s">
+        <v>182</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="33" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="33" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -24317,7 +24304,7 @@
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="33" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -24329,12 +24316,12 @@
     </row>
     <row r="39" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="33" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="30" t="s">
-        <v>156</v>
+      <c r="A40" s="33" t="s">
+        <v>191</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>

</xml_diff>